<commit_message>
Many of changes, added lots of documentation
</commit_message>
<xml_diff>
--- a/Documentatie/Cheery Documentation Planner.xlsx
+++ b/Documentatie/Cheery Documentation Planner.xlsx
@@ -19,6 +19,7 @@
     <definedName name="PeriodInActual">project!A$12=MEDIAN(project!A$12,project!$E1,project!$E1+project!$F1-1)</definedName>
     <definedName name="PeriodInPlan">project!A$12=MEDIAN(project!A$12,project!$C1,project!$C1+project!$D1-1)</definedName>
     <definedName name="Plan">PeriodInPlan*(project!$C1&gt;0)</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">project!$B$2:$CF$20</definedName>
   </definedNames>
   <calcPr calcId="152511" concurrentCalc="0"/>
   <extLst>
@@ -155,16 +156,10 @@
     <t>Basis Ontwerp</t>
   </si>
   <si>
-    <t>DO</t>
-  </si>
-  <si>
     <t>Realisatie</t>
   </si>
   <si>
     <t>Implementatie</t>
-  </si>
-  <si>
-    <t>Fix Period</t>
   </si>
   <si>
     <t>DAYS</t>
@@ -183,6 +178,12 @@
   </si>
   <si>
     <t>Days used:</t>
+  </si>
+  <si>
+    <t>Front-end Detail Design</t>
+  </si>
+  <si>
+    <t>Back-end Detail Design</t>
   </si>
 </sst>
 </file>
@@ -760,7 +761,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp1.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Spin" dx="16" fmlaLink="period_selected" max="60" min="1" page="10" val="11"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Spin" dx="16" fmlaLink="period_selected" max="60" min="1" page="10"/>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1047,41 +1048,23 @@
   </sheetPr>
   <dimension ref="B2:DE41"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="F33" sqref="F33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.75" defaultRowHeight="17.25" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="2.625" customWidth="1"/>
-    <col min="2" max="2" width="15.875" style="2" customWidth="1"/>
+    <col min="2" max="2" width="23.25" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.875" style="1" customWidth="1"/>
     <col min="4" max="4" width="10.125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.375" style="1" customWidth="1"/>
-    <col min="7" max="7" width="7.25" style="7" customWidth="1"/>
+    <col min="5" max="5" width="11.125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="11.375" style="7" customWidth="1"/>
     <col min="8" max="8" width="4.25" style="1" customWidth="1"/>
-    <col min="9" max="28" width="4.875" style="1" customWidth="1"/>
-    <col min="29" max="58" width="4.875" customWidth="1"/>
-    <col min="59" max="59" width="5.25" bestFit="1" customWidth="1"/>
-    <col min="60" max="60" width="5" bestFit="1" customWidth="1"/>
-    <col min="61" max="62" width="5.25" bestFit="1" customWidth="1"/>
-    <col min="63" max="63" width="5.125" bestFit="1" customWidth="1"/>
-    <col min="64" max="64" width="4.25" bestFit="1" customWidth="1"/>
-    <col min="65" max="65" width="4.375" bestFit="1" customWidth="1"/>
-    <col min="66" max="66" width="4.25" bestFit="1" customWidth="1"/>
-    <col min="67" max="67" width="4.375" bestFit="1" customWidth="1"/>
-    <col min="68" max="68" width="4.25" bestFit="1" customWidth="1"/>
-    <col min="69" max="69" width="4.375" bestFit="1" customWidth="1"/>
-    <col min="70" max="70" width="4.125" bestFit="1" customWidth="1"/>
-    <col min="71" max="72" width="4.375" bestFit="1" customWidth="1"/>
-    <col min="73" max="73" width="5.25" bestFit="1" customWidth="1"/>
-    <col min="74" max="74" width="5.125" bestFit="1" customWidth="1"/>
-    <col min="75" max="75" width="5.25" bestFit="1" customWidth="1"/>
-    <col min="76" max="76" width="5.125" bestFit="1" customWidth="1"/>
-    <col min="77" max="77" width="5.25" bestFit="1" customWidth="1"/>
-    <col min="78" max="78" width="5.125" bestFit="1" customWidth="1"/>
-    <col min="79" max="109" width="4.75" customWidth="1"/>
+    <col min="9" max="28" width="5.875" style="1" customWidth="1"/>
+    <col min="29" max="84" width="5.875" customWidth="1"/>
+    <col min="85" max="109" width="4.75" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:109" ht="15" x14ac:dyDescent="0.25">
@@ -1109,7 +1092,7 @@
       <c r="L3" s="8"/>
       <c r="M3" s="8"/>
       <c r="N3" s="9">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="O3" s="8"/>
       <c r="Q3" s="10"/>
@@ -1152,14 +1135,14 @@
     </row>
     <row r="5" spans="2:109" x14ac:dyDescent="0.3">
       <c r="B5" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C5" s="26">
         <f>DATE(2015,10,7)</f>
         <v>42284</v>
       </c>
       <c r="D5" s="28" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E5" s="29">
         <f>DATE(2015,12,15)</f>
@@ -1171,11 +1154,11 @@
     </row>
     <row r="6" spans="2:109" x14ac:dyDescent="0.3">
       <c r="B6" s="2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C6" s="26">
         <f ca="1">NOW()</f>
-        <v>42339.923311226848</v>
+        <v>42348.944510416666</v>
       </c>
       <c r="AT6" s="1"/>
       <c r="AU6" s="1"/>
@@ -1188,11 +1171,11 @@
     </row>
     <row r="8" spans="2:109" x14ac:dyDescent="0.3">
       <c r="B8" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C8" s="27">
         <f ca="1">E5-C6</f>
-        <v>13.076688773151545</v>
+        <v>4.0554895833338378</v>
       </c>
       <c r="AT8" s="1"/>
       <c r="AU8" s="1"/>
@@ -1200,11 +1183,11 @@
     </row>
     <row r="9" spans="2:109" x14ac:dyDescent="0.3">
       <c r="B9" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C9" s="27">
         <f ca="1">C6-C5</f>
-        <v>55.923311226848455</v>
+        <v>64.944510416666162</v>
       </c>
       <c r="I9" s="30">
         <f>C5</f>
@@ -1532,7 +1515,7 @@
       </c>
       <c r="H11" s="4"/>
       <c r="I11" s="4" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="J11" s="4"/>
     </row>
@@ -1897,7 +1880,7 @@
         <v>20</v>
       </c>
       <c r="G14" s="17">
-        <v>0.8</v>
+        <v>0.95</v>
       </c>
       <c r="P14" s="31"/>
       <c r="Q14" s="31"/>
@@ -1940,7 +1923,7 @@
         <v>10</v>
       </c>
       <c r="G15" s="17">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="AJ15" s="31"/>
       <c r="AK15" s="31"/>
@@ -1952,7 +1935,7 @@
     </row>
     <row r="16" spans="2:109" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B16" s="15" t="s">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="C16" s="16">
         <f t="shared" si="4"/>
@@ -1970,12 +1953,12 @@
         <v>10</v>
       </c>
       <c r="G16" s="17">
-        <v>0</v>
+        <v>0.97</v>
       </c>
     </row>
     <row r="17" spans="2:109" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B17" s="15" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="C17" s="16">
         <f t="shared" si="4"/>
@@ -1993,12 +1976,12 @@
         <v>8</v>
       </c>
       <c r="G17" s="17">
-        <v>0</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="18" spans="2:109" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B18" s="15" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C18" s="16">
         <f t="shared" si="4"/>
@@ -2021,7 +2004,7 @@
     </row>
     <row r="19" spans="2:109" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B19" s="15" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C19" s="16">
         <f t="shared" si="4"/>
@@ -2039,7 +2022,7 @@
         <v>5</v>
       </c>
       <c r="G19" s="17">
-        <v>0.2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="20" spans="2:109" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -4330,8 +4313,8 @@
       <formula>FLOOR(I9,1)=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
-  <pageMargins left="0.45" right="0.45" top="0.5" bottom="0.5" header="0.3" footer="0.3"/>
-  <pageSetup scale="42" fitToHeight="0" orientation="landscape" r:id="rId1"/>
+  <pageMargins left="0.43307086614173229" right="0.43307086614173229" top="0.51181102362204722" bottom="0.51181102362204722" header="0.31496062992125984" footer="0.31496062992125984"/>
+  <pageSetup fitToWidth="0" orientation="landscape" r:id="rId1"/>
   <drawing r:id="rId2"/>
   <legacyDrawing r:id="rId3"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">

</xml_diff>